<commit_message>
Removed read me tab from Glider Cal sheets
</commit_message>
<xml_diff>
--- a/CP05MOAS-GL004/Omaha_Cal_Info_CP05MOAS-GL004_00002.xlsx
+++ b/CP05MOAS-GL004/Omaha_Cal_Info_CP05MOAS-GL004_00002.xlsx
@@ -4,18 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="12705" yWindow="-15" windowWidth="12510" windowHeight="12390" tabRatio="377" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="12705" yWindow="-15" windowWidth="12510" windowHeight="12390" tabRatio="377"/>
   </bookViews>
   <sheets>
-    <sheet name="Read Me" sheetId="3" r:id="rId1"/>
-    <sheet name="Moorings" sheetId="1" r:id="rId2"/>
-    <sheet name="Asset_Cal_Info" sheetId="2" r:id="rId3"/>
+    <sheet name="Moorings" sheetId="1" r:id="rId1"/>
+    <sheet name="Asset_Cal_Info" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Asset_Cal_Info!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Asset_Cal_Info!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase">Asset_Cal_Info!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0">Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0">Moorings!$A$1:$J$104</definedName>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Ref Des</t>
   </si>
@@ -75,132 +74,6 @@
   </si>
   <si>
     <t>Deployment Number</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>File Name Instruction</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>:  Convention for naming this file is as follows:</t>
-    </r>
-  </si>
-  <si>
-    <t>Includes:</t>
-  </si>
-  <si>
-    <t>Guidance on data entry</t>
-  </si>
-  <si>
-    <t>Example</t>
-  </si>
-  <si>
-    <t>NOTE:  Delete Guidance and Example prior to submission</t>
-  </si>
-  <si>
-    <t>_v#</t>
-  </si>
-  <si>
-    <t>0000#</t>
-  </si>
-  <si>
-    <t>Version number of this Excel workbook; e.g., v1, v2.</t>
-  </si>
-  <si>
-    <t>NOTE:  Delete Guidance prior to submission</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Asset Cal Info Spreadsheet Instructions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>:  Convention for completing this spreadsheet appears embedded at the bottom of each column on the spreadsheet.</t>
-    </r>
-  </si>
-  <si>
-    <t>Tab names, column names, number formatting must be same format as this sample. This is read by code that is pretty finicky.</t>
-  </si>
-  <si>
-    <t>Readme must be deleted when done</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOTE:  The use of DO NOT CHANGE as guidance in this template is not absolute.  There may be instances where a change is necessary; e.g., an instrument is added/deleted/changed.  Please be careful! </t>
-  </si>
-  <si>
-    <t>Omaha_Cal_Info_CP05MOAS_0000#_v#, where:</t>
-  </si>
-  <si>
-    <r>
-      <t>Unique identifier number</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>/deployment number</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> of a particular CP05MOAS Glider set; e.g., 00001, 00002</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Gliders Spreadsheet Instructions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>:  Convention for completing this spreadsheet is embedded in that spreadsheet.</t>
-    </r>
   </si>
   <si>
     <t>CC_scale_factor1</t>
@@ -267,7 +140,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -292,37 +165,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -376,7 +222,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,25 +237,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,10 +307,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -495,68 +323,58 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="12" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="8" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="12" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -956,126 +774,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="58.28515625" customWidth="1"/>
-    <col min="2" max="2" width="55.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-    </row>
-    <row r="14" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1105,10 +806,10 @@
         <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
@@ -1129,59 +830,59 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="17">
+    <row r="2" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="11">
         <v>387</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="11">
         <v>2</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="12">
         <v>42015</v>
       </c>
-      <c r="E2" s="19">
+      <c r="E2" s="13">
         <v>0.71944444444444444</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="17">
+      <c r="F2" s="12"/>
+      <c r="G2" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="11">
         <v>0</v>
       </c>
-      <c r="J2" s="17" t="str">
+      <c r="J2" s="11" t="str">
         <f>[1]Gliders!J4</f>
         <v>Scarlett Isabella</v>
       </c>
-      <c r="K2" s="18"/>
-      <c r="L2" s="33">
+      <c r="K2" s="12"/>
+      <c r="L2" s="27">
         <f>((LEFT(G2,(FIND("°",G2,1)-1)))+(MID(G2,(FIND("°",G2,1)+1),(FIND("'",G2,1))-(FIND("°",G2,1)+1))/60))*(IF(RIGHT(G2,1)="N",1,-1))</f>
         <v>40.008650000000003</v>
       </c>
-      <c r="M2" s="33">
+      <c r="M2" s="27">
         <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="E",1,-1))</f>
         <v>-70.399833333333333</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="5"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="A6" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1189,11 +890,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
@@ -1216,7 +917,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>11</v>
@@ -1227,383 +928,383 @@
       <c r="E1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="23">
+      <c r="A2" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="17">
         <v>387</v>
       </c>
-      <c r="C2" s="23">
+      <c r="C2" s="17">
         <v>2</v>
       </c>
-      <c r="D2" s="28">
+      <c r="D2" s="22">
         <v>654587</v>
       </c>
-      <c r="E2" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="30">
+      <c r="E2" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="24">
         <v>0.61</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="23">
+      <c r="A3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="17">
         <v>387</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="17">
         <v>2</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="22">
         <v>654587</v>
       </c>
-      <c r="E3" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="30">
+      <c r="E3" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="24">
         <v>0.61</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="23">
+      <c r="A4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="17">
         <v>387</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="17">
         <v>2</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="22">
         <v>654587</v>
       </c>
-      <c r="E4" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="30">
+      <c r="E4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="24">
         <v>0.61</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="23">
+      <c r="A5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="17">
         <v>387</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="17">
         <v>2</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="22">
         <v>654587</v>
       </c>
-      <c r="E5" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="30">
+      <c r="E5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="24">
         <v>0.61</v>
       </c>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-    </row>
-    <row r="7" spans="1:16" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="23">
+      <c r="A6" s="9"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+    </row>
+    <row r="7" spans="1:16" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="17">
         <v>387</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="17">
         <v>2</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="22">
         <v>3190</v>
       </c>
-      <c r="E7" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="31">
+      <c r="E7" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="25">
         <v>124</v>
       </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-    </row>
-    <row r="8" spans="1:16" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="23">
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" spans="1:16" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="17">
         <v>387</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="17">
         <v>2</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="22">
         <v>3190</v>
       </c>
-      <c r="E8" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="31">
+      <c r="E8" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="25">
         <v>700</v>
       </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-    </row>
-    <row r="9" spans="1:16" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="23">
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" spans="1:16" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="17">
         <v>387</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="17">
         <v>2</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="22">
         <v>3190</v>
       </c>
-      <c r="E9" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="31">
+      <c r="E9" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="25">
         <v>1.0760000000000001</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-    </row>
-    <row r="10" spans="1:16" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="23">
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+    </row>
+    <row r="10" spans="1:16" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="17">
         <v>387</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="17">
         <v>2</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="22">
         <v>3190</v>
       </c>
-      <c r="E10" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="31">
+      <c r="E10" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="25">
         <v>3.9E-2</v>
       </c>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-    </row>
-    <row r="11" spans="1:16" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-    </row>
-    <row r="12" spans="1:16" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="23">
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="1:16" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="9"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="1:16" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="17">
         <v>387</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="17">
         <v>2</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="22">
         <v>9087</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-    </row>
-    <row r="13" spans="1:16" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="20"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-    </row>
-    <row r="14" spans="1:16" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="23">
+      <c r="E12" s="15"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+    </row>
+    <row r="13" spans="1:16" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="14"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+    </row>
+    <row r="14" spans="1:16" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="17">
         <v>387</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="17">
         <v>2</v>
       </c>
-      <c r="D14" s="28">
+      <c r="D14" s="22">
         <v>173</v>
       </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-    </row>
-    <row r="15" spans="1:16" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="20"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-    </row>
-    <row r="16" spans="1:16" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="23">
+      <c r="E14" s="15"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+    </row>
+    <row r="15" spans="1:16" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="14"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" spans="1:16" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="17">
         <v>387</v>
       </c>
-      <c r="C16" s="23">
+      <c r="C16" s="17">
         <v>2</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D16" s="22">
         <v>50165</v>
       </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-    </row>
-    <row r="17" spans="1:11" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-    </row>
-    <row r="18" spans="1:11" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="23">
+      <c r="E16" s="15"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+    </row>
+    <row r="17" spans="1:11" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="14"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+    </row>
+    <row r="18" spans="1:11" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="17">
         <v>387</v>
       </c>
-      <c r="C18" s="23">
+      <c r="C18" s="17">
         <v>2</v>
       </c>
-      <c r="D18" s="28">
+      <c r="D18" s="22">
         <v>387</v>
       </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>